<commit_message>
Nueva tarea en el productBacklog
</commit_message>
<xml_diff>
--- a/Documentacion/scrum.xlsx
+++ b/Documentacion/scrum.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
   <si>
     <t>Product Backlog Items-Prototipo de Realidad Aumentada</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>Diseño y implementacion de interfaz para agregar un modelo 3d</t>
+  </si>
+  <si>
+    <t>Ejecutar un ejemplo de Prueba e instalar en apk</t>
   </si>
 </sst>
 </file>
@@ -388,6 +391,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -417,18 +432,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -724,10 +727,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -740,13 +743,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="23"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:5" ht="30.75" thickBot="1">
       <c r="A2" s="1" t="s">
@@ -766,7 +769,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A3" s="31">
+      <c r="A3" s="21">
         <v>1</v>
       </c>
       <c r="B3" s="17" t="s">
@@ -774,72 +777,76 @@
       </c>
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
-      <c r="E3" s="32"/>
+      <c r="E3" s="22"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A4" s="33">
+      <c r="A4" s="21">
         <v>2</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A5" s="21">
+        <v>3</v>
+      </c>
+      <c r="B5" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A5" s="33">
-        <v>3</v>
-      </c>
-      <c r="B5" s="34" t="s">
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A6" s="21">
+        <v>4</v>
+      </c>
+      <c r="B6" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A6" s="33">
-        <v>4</v>
-      </c>
-      <c r="B6" s="34" t="s">
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A7" s="21">
+        <v>5</v>
+      </c>
+      <c r="B7" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A7" s="33">
-        <v>5</v>
-      </c>
-      <c r="B7" s="34" t="s">
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A8" s="21">
+        <v>6</v>
+      </c>
+      <c r="B8" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A8" s="33">
-        <v>6</v>
-      </c>
-      <c r="B8" s="34" t="s">
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A9" s="21">
+        <v>7</v>
+      </c>
+      <c r="B9" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A9" s="33"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A10" s="16"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>
@@ -847,14 +854,14 @@
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1">
       <c r="A11" s="16"/>
-      <c r="B11" s="17"/>
+      <c r="B11" s="24"/>
       <c r="C11" s="17"/>
       <c r="D11" s="17"/>
       <c r="E11" s="17"/>
     </row>
     <row r="12" spans="1:5" ht="15.75" thickBot="1">
       <c r="A12" s="16"/>
-      <c r="B12" s="34"/>
+      <c r="B12" s="17"/>
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
       <c r="E12" s="17"/>
@@ -903,17 +910,16 @@
     </row>
     <row r="19" spans="1:5" ht="15.75" thickBot="1">
       <c r="A19" s="16"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="14"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A20" s="16"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -944,15 +950,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="23"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="27"/>
     </row>
     <row r="2" spans="1:7" ht="30.75" thickBot="1">
       <c r="A2" s="1" t="s">
@@ -989,7 +995,7 @@
       <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="29" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="5"/>
@@ -1000,7 +1006,7 @@
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A5" s="27"/>
+      <c r="A5" s="31"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -1009,7 +1015,7 @@
       <c r="G5" s="5"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A6" s="27"/>
+      <c r="A6" s="31"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -1018,7 +1024,7 @@
       <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A7" s="27"/>
+      <c r="A7" s="31"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -1027,7 +1033,7 @@
       <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A8" s="27"/>
+      <c r="A8" s="31"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -1036,7 +1042,7 @@
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A9" s="27"/>
+      <c r="A9" s="31"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -1045,7 +1051,7 @@
       <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A10" s="28"/>
+      <c r="A10" s="32"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6" t="s">
         <v>11</v>
@@ -1070,7 +1076,7 @@
       <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="28" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="3"/>
@@ -1081,7 +1087,7 @@
       <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A13" s="25"/>
+      <c r="A13" s="29"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -1090,7 +1096,7 @@
       <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A14" s="25"/>
+      <c r="A14" s="29"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -1099,7 +1105,7 @@
       <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A15" s="25"/>
+      <c r="A15" s="29"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -1108,7 +1114,7 @@
       <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A16" s="25"/>
+      <c r="A16" s="29"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -1117,7 +1123,7 @@
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A17" s="25"/>
+      <c r="A17" s="29"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -1126,7 +1132,7 @@
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A18" s="25"/>
+      <c r="A18" s="29"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -1135,7 +1141,7 @@
       <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A19" s="26"/>
+      <c r="A19" s="30"/>
       <c r="B19" s="5"/>
       <c r="C19" s="6" t="s">
         <v>11</v>
@@ -1179,12 +1185,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="24" thickBot="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
     </row>
     <row r="2" spans="1:4" ht="20.25" thickBot="1">
       <c r="A2" s="7" t="s">
@@ -1232,13 +1238,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="23"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:5" ht="30">
       <c r="A2" s="12" t="s">

</xml_diff>

<commit_message>
Arreglo del mensaje de error del archivo de scrum
</commit_message>
<xml_diff>
--- a/Documentacion/scrum.xlsx
+++ b/Documentacion/scrum.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Retrospective" sheetId="3" r:id="rId3"/>
     <sheet name="Hoja1" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725" iterateDelta="1E-4"/>
+  <calcPr calcId="124519" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -295,12 +295,6 @@
   </cellStyleXfs>
   <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -332,16 +326,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -708,7 +708,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
       <selection activeCell="A7" sqref="A7:B9"/>
     </sheetView>
   </sheetViews>
@@ -723,191 +723,191 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
     </row>
     <row r="2" spans="1:5" ht="30.75" customHeight="1">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A3" s="10">
+      <c r="A3" s="8">
         <v>1</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="11">
+      <c r="C3" s="10"/>
+      <c r="D3" s="9">
         <v>3</v>
       </c>
-      <c r="E3" s="10"/>
+      <c r="E3" s="8"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A4" s="10">
+      <c r="A4" s="8">
         <v>2</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="13">
+      <c r="C4" s="10"/>
+      <c r="D4" s="11">
         <v>2</v>
       </c>
-      <c r="E4" s="13"/>
+      <c r="E4" s="11"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A5" s="10">
+      <c r="A5" s="8">
         <v>3</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="13">
+      <c r="C5" s="10"/>
+      <c r="D5" s="11">
         <v>3</v>
       </c>
-      <c r="E5" s="13"/>
+      <c r="E5" s="11"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A6" s="17">
+      <c r="A6" s="13">
         <v>4</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12">
+      <c r="C6" s="10"/>
+      <c r="D6" s="10">
         <v>5</v>
       </c>
-      <c r="E6" s="13"/>
+      <c r="E6" s="11"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A7" s="10">
+      <c r="A7" s="8">
         <v>5</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="13">
+      <c r="C7" s="10"/>
+      <c r="D7" s="11">
         <v>4</v>
       </c>
-      <c r="E7" s="13"/>
+      <c r="E7" s="11"/>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A8" s="10">
+      <c r="A8" s="8">
         <v>6</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="13">
+      <c r="C8" s="10"/>
+      <c r="D8" s="11">
         <v>6</v>
       </c>
-      <c r="E8" s="11"/>
+      <c r="E8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A9" s="10">
+      <c r="A9" s="8">
         <v>7</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="11">
+      <c r="C9" s="10"/>
+      <c r="D9" s="9">
         <v>8</v>
       </c>
-      <c r="E9" s="11"/>
+      <c r="E9" s="9"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A10" s="11"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A15" s="11"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A18" s="11"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
+      <c r="A18" s="9"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A19" s="11"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
+      <c r="A19" s="9"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -922,8 +922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -941,57 +941,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" thickTop="1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
     </row>
     <row r="2" spans="1:7" ht="30.75" customHeight="1">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="12" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="8">
         <v>1</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="9">
         <v>6</v>
       </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11" t="s">
+      <c r="E3" s="9"/>
+      <c r="F3" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="9" t="s">
         <v>29</v>
       </c>
     </row>
@@ -999,199 +999,196 @@
       <c r="A4" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="8">
         <v>2</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="9">
         <v>8</v>
       </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11" t="s">
+      <c r="E4" s="9"/>
+      <c r="F4" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="9" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="16"/>
-      <c r="B5" s="10">
+      <c r="B5" s="8">
         <v>3</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="9">
         <v>6</v>
       </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11" t="s">
+      <c r="E5" s="9"/>
+      <c r="F5" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="11"/>
+      <c r="G5" s="9"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="16"/>
-      <c r="B6" s="10">
+      <c r="B6" s="8">
         <v>4</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="9">
         <v>10</v>
       </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11" t="s">
+      <c r="E6" s="9"/>
+      <c r="F6" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="11"/>
+      <c r="G6" s="9"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" s="16"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" s="16"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" s="16"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" s="16"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12" t="s">
+      <c r="B10" s="10"/>
+      <c r="C10" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="10">
         <f>SUM(D3:D9)</f>
         <v>30</v>
       </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="11"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="9"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="11"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="9"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="A12" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="8">
         <v>5</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="A13" s="16"/>
-      <c r="B13" s="10">
+      <c r="B13" s="8">
         <v>6</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" s="16"/>
-      <c r="B14" s="10">
+      <c r="B14" s="8">
         <v>7</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="A15" s="16"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="A16" s="16"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="A17" s="16"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="A18" s="16"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="A19" s="16"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="12" t="s">
+      <c r="B19" s="9"/>
+      <c r="C19" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="12">
-        <f ca="1">SUM(D12:D19)</f>
-        <v>0</v>
-      </c>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1222,34 +1219,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="24" customHeight="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
     </row>
     <row r="2" spans="1:4" ht="20.25" customHeight="1">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="48" customHeight="1">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="7"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1278,28 +1275,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="7" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>